<commit_message>
Group Project - Penetration Testing Scenario
</commit_message>
<xml_diff>
--- a/Group_Contributions.xlsx
+++ b/Group_Contributions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenne\Documents\Uni\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A0828A-2A2B-45D8-8038-45E546019A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFA4E8E-266F-4032-AC4E-C72B3B067EAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9540" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Week</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Project manager</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -67,6 +64,12 @@
   </si>
   <si>
     <t>Jake</t>
+  </si>
+  <si>
+    <t>Kenneth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          01/03/2021</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +90,12 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -544,17 +553,17 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -562,30 +571,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6">
         <v>44221</v>
@@ -594,166 +603,301 @@
         <v>0.16666666666666599</v>
       </c>
       <c r="D2" s="2">
-        <v>0.16666666666666599</v>
+        <v>0.10666666666666599</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16666666666666599</v>
+        <v>0.28666666666666601</v>
       </c>
       <c r="F2" s="2">
         <v>0.16666666666666599</v>
       </c>
       <c r="G2" s="2">
-        <v>0.16666666666666599</v>
+        <v>0.10666666666666599</v>
       </c>
       <c r="H2" s="2">
         <v>0.16666666666666599</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(C2:H2)</f>
-        <v>0.99999999999999589</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6">
         <v>44228</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="C3" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.28666666666666601</v>
+      </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J13" si="0">SUM(C3:H3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>44235</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.13666666666666599</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.13666666666666599</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.16666666666666599</v>
+      </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>44242</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.16666666666666599</v>
+      </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.99999999999999589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>44249</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.10666666666666599</v>
+      </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.10666666666666599</v>
+      </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>44263</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.10666666666666599</v>
+      </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>44270</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.22666666666666599</v>
+      </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>44277</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.16666666666666599</v>
+      </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.99999999999999589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>44284</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.10666666666666599</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.22666666666666599</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.16666666666666599</v>
+      </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>44305</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -766,9 +910,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>44312</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -781,28 +928,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
         <f>SUM(C2:C13)/COUNT(C2:C13)</f>
-        <v>0.16666666666666599</v>
+        <v>0.16066666666666601</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:J15" si="1">SUM(D2:D13)/COUNT(D2:D13)</f>
-        <v>0.16666666666666599</v>
+        <v>0.15166666666666601</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>0.16666666666666599</v>
+        <v>0.17566666666666603</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0.16666666666666599</v>
+        <v>0.178666666666666</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
@@ -810,14 +957,15 @@
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>0.16666666666666599</v>
+        <v>0.16666666666666602</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="1"/>
-        <v>8.3333333333332996E-2</v>
+        <v>0.83333333333333026</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>